<commit_message>
califonia knows how to party (str_replace_all to california)
</commit_message>
<xml_diff>
--- a/curation/invert_counts_curated.xlsx
+++ b/curation/invert_counts_curated.xlsx
@@ -402,7 +402,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>califonia cone snail</t>
+          <t>california cone snail</t>
         </is>
       </c>
       <c r="D2">
@@ -532,7 +532,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>califonia cone snail</t>
+          <t>california cone snail</t>
         </is>
       </c>
       <c r="D7">
@@ -662,7 +662,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>califonia cone snail</t>
+          <t>california cone snail</t>
         </is>
       </c>
       <c r="D12">
@@ -792,7 +792,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>califonia cone snail</t>
+          <t>california cone snail</t>
         </is>
       </c>
       <c r="D17">
@@ -907,7 +907,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>califonia cone snail</t>
+          <t>california cone snail</t>
         </is>
       </c>
       <c r="D22">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>califonia cone snail</t>
+          <t>california cone snail</t>
         </is>
       </c>
       <c r="D27">
@@ -1167,7 +1167,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>califonia cone snail</t>
+          <t>california cone snail</t>
         </is>
       </c>
       <c r="D32">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>califonia cone snail</t>
+          <t>california cone snail</t>
         </is>
       </c>
       <c r="D37">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>califonia cone snail</t>
+          <t>california cone snail</t>
         </is>
       </c>
       <c r="D42">
@@ -1557,7 +1557,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>califonia cone snail</t>
+          <t>california cone snail</t>
         </is>
       </c>
       <c r="D47">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>califonia cone snail</t>
+          <t>california cone snail</t>
         </is>
       </c>
       <c r="D52">

</xml_diff>